<commit_message>
feat(filters): Add `merge` option in `dict` filter.
</commit_message>
<xml_diff>
--- a/tests/files/excel.xlsx
+++ b/tests/files/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/xlreader/tests/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/xlref/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4712F826-D4C9-EB4B-8663-F9B8B31D6E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4006ABA-A734-5D46-9673-B4CEDCBA267D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{47B895AD-9ED1-804B-9EDF-D266AD47F035}"/>
+    <workbookView xWindow="5560" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{47B895AD-9ED1-804B-9EDF-D266AD47F035}"/>
   </bookViews>
   <sheets>
     <sheet name="origin" sheetId="2" r:id="rId1"/>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>c</t>
   </si>
@@ -175,10 +169,22 @@
     <t>test.xlsx#Sheet2!^^:__</t>
   </si>
   <si>
-    <t>#ref!A1(RD):._:R[{"fun":"dict","key":"upper","value":"ref"}]</t>
-  </si>
-  <si>
     <t>#E_(U):_^</t>
+  </si>
+  <si>
+    <t>#ref!A1(RD):._:R[{"fun":"dict","key":"upper","value":"ref","merge":true}]</t>
+  </si>
+  <si>
+    <t>merge-1</t>
+  </si>
+  <si>
+    <t>merge-2</t>
+  </si>
+  <si>
+    <t>#B1</t>
+  </si>
+  <si>
+    <t>#origin!A3:B4["recursive", "dict"]</t>
   </si>
 </sst>
 </file>
@@ -536,20 +542,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821277F2-6EA5-8A4F-AF1F-E2D1D709B252}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -559,10 +581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841A364C-9194-D54E-9C8A-8F64F7557C4F}">
-  <dimension ref="B2:O24"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -785,7 +807,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -866,6 +888,11 @@
       </c>
       <c r="C24" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(filters): Remove `merge` option in `dict` filter and add list filters for `key` and `value` options.
</commit_message>
<xml_diff>
--- a/tests/files/excel.xlsx
+++ b/tests/files/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/xlref/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4006ABA-A734-5D46-9673-B4CEDCBA267D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7001F176-D1F6-5D4B-800A-B3CCEF9242D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{47B895AD-9ED1-804B-9EDF-D266AD47F035}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>#E_(U):_^</t>
   </si>
   <si>
-    <t>#ref!A1(RD):._:R[{"fun":"dict","key":"upper","value":"ref","merge":true}]</t>
-  </si>
-  <si>
     <t>merge-1</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>#origin!A3:B4["recursive", "dict"]</t>
+  </si>
+  <si>
+    <t>#ref!A1(RD):._:R[{"fun":"dict","key":"ref","value":"ref"},{"fun":"dict","key":["upper"]}]</t>
   </si>
 </sst>
 </file>
@@ -545,14 +545,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -568,10 +568,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +892,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(test): Add new test cases.
</commit_message>
<xml_diff>
--- a/tests/files/excel.xlsx
+++ b/tests/files/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/xlref/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7001F176-D1F6-5D4B-800A-B3CCEF9242D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D46D417-D947-FE48-BBF4-80879E95426B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{47B895AD-9ED1-804B-9EDF-D266AD47F035}"/>
+    <workbookView xWindow="5560" yWindow="1400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{47B895AD-9ED1-804B-9EDF-D266AD47F035}"/>
   </bookViews>
   <sheets>
     <sheet name="origin" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>c</t>
   </si>
@@ -185,13 +185,31 @@
   </si>
   <si>
     <t>#ref!A1(RD):._:R[{"fun":"dict","key":"ref","value":"ref"},{"fun":"dict","key":["upper"]}]</t>
+  </si>
+  <si>
+    <t>expand-8</t>
+  </si>
+  <si>
+    <t>#P4:RR</t>
+  </si>
+  <si>
+    <t>expand-9</t>
+  </si>
+  <si>
+    <t>#P30:Q31:RR</t>
+  </si>
+  <si>
+    <t>expand-10</t>
+  </si>
+  <si>
+    <t>#M7:Q7:RRRRD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -544,13 +562,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821277F2-6EA5-8A4F-AF1F-E2D1D709B252}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -558,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -566,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -581,15 +599,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841A364C-9194-D54E-9C8A-8F64F7557C4F}">
-  <dimension ref="B2:O25"/>
+  <dimension ref="B2:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -612,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -632,7 +650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -655,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -663,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -680,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -712,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -738,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -770,7 +788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -778,7 +796,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -786,7 +804,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -794,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -802,96 +820,120 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
-      <c r="B15" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
-      <c r="B16" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
-      <c r="B20" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
-      <c r="B25" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>